<commit_message>
v2p10. Added Double Lane Change ISO3888, CRG Hockenheim. Configurable steering wheel (FSAE, Sedan).
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Steer/Ackermann/sm_car_data_Steer_Ackermann.xlsx
+++ b/Libraries/Vehicle/Steer/Ackermann/sm_car_data_Steer_Ackermann.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Vehicle\Steer\Ackermann\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\ssvt\Libraries\Vehicle\Steer\Ackermann\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD502B64-E251-49DF-A119-4740F9C6DFD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889776E9-5E44-46A5-A19C-C9827C4102C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" tabRatio="717" activeTab="5" xr2:uid="{6551A3D7-48D1-475C-90BB-3A0F5E8315B3}"/>
+    <workbookView xWindow="2865" yWindow="1185" windowWidth="20700" windowHeight="10110" tabRatio="717" xr2:uid="{6551A3D7-48D1-475C-90BB-3A0F5E8315B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sedan_Hamba_f" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="33">
   <si>
     <t>Units</t>
   </si>
@@ -135,6 +135,9 @@
   <si>
     <t>Vehicle.Chassis.Body.sAxle1.Value - Vehicle.Chassis.Body.sAxle(rear).Value</t>
   </si>
+  <si>
+    <t>Sedan</t>
+  </si>
 </sst>
 </file>
 
@@ -198,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -231,11 +234,78 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="67">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -955,28 +1025,28 @@
   <sheetPr>
     <tabColor rgb="FFFF9999"/>
   </sheetPr>
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -996,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1027,7 +1097,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1041,7 +1111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1055,7 +1125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1068,7 +1138,7 @@
         <v>0.35809000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1109,7 +1179,7 @@
       <c r="AA6"/>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>14</v>
@@ -1144,7 +1214,7 @@
       <c r="AA7"/>
       <c r="AB7"/>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>13</v>
@@ -1182,64 +1252,59 @@
       <c r="AA8"/>
       <c r="AB8"/>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15">
-        <v>100</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-    </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7">
-        <v>2.8239999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15">
+        <v>100</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+    </row>
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1247,70 +1312,78 @@
         <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7">
+        <v>2.8239999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7">
         <f>0.7865*2</f>
         <v>1.573</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="6"/>
@@ -1320,59 +1393,79 @@
       <c r="G20" s="6"/>
       <c r="H20" s="13"/>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="13"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A15:B16 A4:B4">
-    <cfRule type="cellIs" dxfId="57" priority="10" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:B18">
-    <cfRule type="cellIs" dxfId="56" priority="11" operator="equal">
+  <conditionalFormatting sqref="A16:B17 A4:B4">
+    <cfRule type="cellIs" dxfId="66" priority="12" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:B19">
+    <cfRule type="cellIs" dxfId="65" priority="13" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="cellIs" dxfId="64" priority="10" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="cellIs" dxfId="55" priority="8" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="54" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B7">
-    <cfRule type="cellIs" dxfId="53" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:B8">
-    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="58" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="cellIs" dxfId="56" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:B9">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1395,18 +1488,18 @@
       <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1426,7 +1519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1457,7 +1550,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1471,7 +1564,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1485,7 +1578,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1498,7 +1591,7 @@
         <v>0.35809000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1535,7 +1628,7 @@
       <c r="AA6"/>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
@@ -1553,7 +1646,7 @@
         <v>2.8239999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -1572,51 +1665,51 @@
         <v>1.573</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="6"/>
@@ -1626,7 +1719,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="6"/>
@@ -1638,37 +1731,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B13 A4:B4">
-    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="10" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:B15">
-    <cfRule type="cellIs" dxfId="45" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="11" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="44" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="43" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="9" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1681,28 +1774,28 @@
   <sheetPr>
     <tabColor rgb="FFFF9999"/>
   </sheetPr>
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1722,7 +1815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1753,7 +1846,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1767,7 +1860,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1781,7 +1874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1794,7 +1887,7 @@
         <v>0.35809000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1835,7 +1928,7 @@
       <c r="AA6"/>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>14</v>
@@ -1870,7 +1963,7 @@
       <c r="AA7"/>
       <c r="AB7"/>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>13</v>
@@ -1908,64 +2001,59 @@
       <c r="AA8"/>
       <c r="AB8"/>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15">
-        <v>100</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-    </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7">
-        <v>3.57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15">
+        <v>100</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+    </row>
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1973,70 +2061,78 @@
         <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7">
         <f>0.9921*2</f>
         <v>1.9842</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="6"/>
@@ -2046,59 +2142,79 @@
       <c r="G20" s="6"/>
       <c r="H20" s="13"/>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="13"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A15:B16 A4:B4">
-    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:B18">
-    <cfRule type="cellIs" dxfId="38" priority="11" operator="equal">
+  <conditionalFormatting sqref="A16:B17 A4:B4">
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:B19">
+    <cfRule type="cellIs" dxfId="45" priority="13" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B7">
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:B8">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:B9">
+    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2118,21 +2234,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2152,7 +2268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2183,7 +2299,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2197,7 +2313,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2211,7 +2327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -2224,7 +2340,7 @@
         <v>0.35809000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -2261,7 +2377,7 @@
       <c r="AA6"/>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
@@ -2279,7 +2395,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -2298,51 +2414,51 @@
         <v>1.9842</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="6"/>
@@ -2352,7 +2468,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="6"/>
@@ -2364,37 +2480,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B13 A4:B4">
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:B15">
-    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="9" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2407,28 +2523,28 @@
   <sheetPr>
     <tabColor rgb="FFFF9999"/>
   </sheetPr>
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2448,7 +2564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2479,7 +2595,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2493,7 +2609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2507,7 +2623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -2520,7 +2636,7 @@
         <v>0.35809000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -2561,7 +2677,7 @@
       <c r="AA6"/>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>14</v>
@@ -2596,7 +2712,7 @@
       <c r="AA7"/>
       <c r="AB7"/>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>13</v>
@@ -2634,64 +2750,59 @@
       <c r="AA8"/>
       <c r="AB8"/>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15">
-        <v>100</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-    </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7">
-        <v>6.7816159999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15">
+        <v>100</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+    </row>
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2699,70 +2810,78 @@
         <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7">
+        <v>6.7816159999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7">
         <f>0.83834*2</f>
         <v>1.6766799999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="6"/>
@@ -2772,59 +2891,79 @@
       <c r="G20" s="6"/>
       <c r="H20" s="13"/>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="13"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A15:B16 A4:B4">
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:B18">
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+  <conditionalFormatting sqref="A16:B17 A4:B4">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:B19">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B7">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:B8">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:B9">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2837,28 +2976,28 @@
   <sheetPr>
     <tabColor rgb="FFFF9999"/>
   </sheetPr>
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2878,7 +3017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2909,7 +3048,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -2923,7 +3062,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2937,7 +3076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -2950,7 +3089,7 @@
         <v>0.35809000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -2991,7 +3130,7 @@
       <c r="AA6"/>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>14</v>
@@ -3026,7 +3165,7 @@
       <c r="AA7"/>
       <c r="AB7"/>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>13</v>
@@ -3064,64 +3203,59 @@
       <c r="AA8"/>
       <c r="AB8"/>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15">
-        <v>100</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-    </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7">
-        <v>6.4820000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15">
+        <v>100</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+    </row>
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3129,70 +3263,78 @@
         <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7">
+        <v>6.4820000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7">
         <f>0.96035*2</f>
         <v>1.9207000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="6"/>
@@ -3202,59 +3344,79 @@
       <c r="G20" s="6"/>
       <c r="H20" s="13"/>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="13"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A15:B16 A4:B4">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:B18">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+  <conditionalFormatting sqref="A16:B17 A4:B4">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:B19">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B7">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:B8">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:B9">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>